<commit_message>
v0.7.0.0 alpha. Aibe and Aiwe now support localization!
</commit_message>
<xml_diff>
--- a/AIWE Table Making Guideline v20171006.xlsx
+++ b/AIWE Table Making Guideline v20171006.xlsx
@@ -3313,6 +3313,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <u/>
       <sz val="11"/>
@@ -3337,36 +3367,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -3437,7 +3437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3471,80 +3471,78 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4148,639 +4146,639 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="76.6640625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="127.77734375" style="27" customWidth="1"/>
-    <col min="5" max="5" width="98.77734375" style="28" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="26"/>
+    <col min="1" max="1" width="4.109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="76.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="127.77734375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="98.77734375" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="18" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="24" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="33">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37">
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29">
         <v>2</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="33">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="33">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="33">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="30" t="s">
         <v>514</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="37">
+      <c r="A8" s="29">
         <v>6</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="31" t="s">
         <v>506</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="33">
+      <c r="A9" s="25">
         <v>7</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="30" t="s">
         <v>515</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="33">
+      <c r="A10" s="25">
         <v>8</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="31" t="s">
         <v>507</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="36"/>
-    </row>
-    <row r="11" spans="1:5" s="27" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="33">
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
         <v>9</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="36"/>
-    </row>
-    <row r="12" spans="1:5" s="27" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A12" s="37">
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" s="19" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A12" s="29">
         <v>10</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="31" t="s">
         <v>508</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="32" t="s">
         <v>724</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="32" t="s">
         <v>725</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="33" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="33">
+    <row r="13" spans="1:5" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
         <v>11</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="33">
+      <c r="A14" s="25">
         <v>12</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="36"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="33">
+      <c r="A15" s="25">
         <v>13</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="31" t="s">
         <v>509</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="32" t="s">
         <v>472</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="36"/>
-    </row>
-    <row r="16" spans="1:5" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="37">
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5" s="19" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="29">
         <v>14</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="32" t="s">
         <v>516</v>
       </c>
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="1:5" s="27" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="33">
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
         <v>15</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="1:5" s="27" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="33">
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" s="19" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
         <v>16</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="30" t="s">
         <v>517</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="34" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="33">
+      <c r="A19" s="25">
         <v>17</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="36"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="37">
+      <c r="A20" s="29">
         <v>18</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="30" t="s">
         <v>518</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="33">
+      <c r="A21" s="25">
         <v>19</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="33">
+      <c r="A22" s="25">
         <v>20</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="33">
+      <c r="A23" s="25">
         <v>21</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="30" t="s">
         <v>519</v>
       </c>
-      <c r="E23" s="36"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="37">
+      <c r="A24" s="29">
         <v>22</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="35" t="s">
         <v>520</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="33">
+      <c r="A25" s="25">
         <v>23</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="31" t="s">
         <v>510</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="30" t="s">
         <v>521</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="34" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="33">
+      <c r="A26" s="25">
         <v>24</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="30" t="s">
         <v>522</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="28" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="144" x14ac:dyDescent="0.3">
-      <c r="A27" s="33">
+      <c r="A27" s="25">
         <v>25</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="32" t="s">
         <v>538</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="34" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37">
+    <row r="28" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="29">
         <v>26</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="27" t="s">
         <v>532</v>
       </c>
-      <c r="E28" s="36"/>
-    </row>
-    <row r="29" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="33">
+      <c r="E28" s="28"/>
+    </row>
+    <row r="29" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
         <v>27</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="27" t="s">
         <v>533</v>
       </c>
-      <c r="E29" s="36"/>
-    </row>
-    <row r="30" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33">
+      <c r="E29" s="28"/>
+    </row>
+    <row r="30" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
         <v>28</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="32" t="s">
         <v>666</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="32" t="s">
         <v>666</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="32" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="27" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="33">
+    <row r="31" spans="1:5" s="19" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
         <v>29</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="27" t="s">
         <v>511</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="30" t="s">
         <v>523</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="34" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37">
+    <row r="32" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="29">
         <v>30</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="E32" s="36"/>
-    </row>
-    <row r="33" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37">
+      <c r="E32" s="28"/>
+    </row>
+    <row r="33" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="29">
         <v>31</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="1:5" s="27" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A34" s="37">
+      <c r="E33" s="28"/>
+    </row>
+    <row r="34" spans="1:5" s="19" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A34" s="29">
         <v>32</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="30" t="s">
         <v>524</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="34" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="49" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="45">
+    <row r="35" spans="1:5" s="41" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="37">
         <v>33</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="38" t="s">
         <v>525</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="39" t="s">
         <v>528</v>
       </c>
-      <c r="E35" s="48"/>
-    </row>
-    <row r="36" spans="1:5" s="49" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="45">
+      <c r="E35" s="40"/>
+    </row>
+    <row r="36" spans="1:5" s="41" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="37">
         <v>34</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="38" t="s">
         <v>526</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="39" t="s">
         <v>527</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="39" t="s">
         <v>529</v>
       </c>
-      <c r="E36" s="48"/>
-    </row>
-    <row r="37" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="45">
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="1:5" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="37">
         <v>35</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="38" t="s">
         <v>530</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="47" t="s">
+      <c r="D37" s="39" t="s">
         <v>531</v>
       </c>
-      <c r="E37" s="48"/>
-    </row>
-    <row r="38" spans="1:5" s="49" customFormat="1" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="45">
+      <c r="E37" s="40"/>
+    </row>
+    <row r="38" spans="1:5" s="41" customFormat="1" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="37">
         <v>36</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="38" t="s">
         <v>542</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="39" t="s">
         <v>545</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="D38" s="39" t="s">
         <v>547</v>
       </c>
-      <c r="E38" s="48" t="s">
+      <c r="E38" s="40" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="49" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="45">
+    <row r="39" spans="1:5" s="41" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="37">
         <v>37</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="38" t="s">
         <v>543</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="39" t="s">
         <v>544</v>
       </c>
-      <c r="D39" s="47" t="s">
+      <c r="D39" s="39" t="s">
         <v>546</v>
       </c>
-      <c r="E39" s="48" t="s">
+      <c r="E39" s="40" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="26" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="38" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="31" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="51" t="s">
+      <c r="B46" s="43" t="s">
         <v>308</v>
       </c>
     </row>
@@ -4794,1013 +4792,1005 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA577669-2296-4A56-8D5E-0E7677CCC01C}">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="14" width="2.77734375" style="19" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="19"/>
+    <col min="1" max="14" width="2.77734375" style="45" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="44" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="45" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="45" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="45" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="45" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="45" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="45" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="46" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="46" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="46" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="46" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="45" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="45" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="45" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="45" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="22" t="s">
+    <row r="17" spans="1:5" s="47" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="48" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="44" t="s">
         <v>609</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="49"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="45" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="46" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="45" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="46" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="45" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="45" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="46" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="45" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="45" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="45" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="45" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="50" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="45" t="s">
         <v>722</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="50"/>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="50" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="45" t="s">
         <v>721</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="50"/>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="50" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="45" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="45" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="50" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="45" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="45" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="45" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="45" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F43" s="19" t="s">
+      <c r="F43" s="45" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="45" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="45" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="45" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="45" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="45" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="46" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="45" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="45" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="50" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="19" t="s">
+      <c r="E53" s="45" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="45" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="45" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="45" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="45" t="s">
         <v>559</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="G57" s="45" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F58" s="19" t="s">
+      <c r="F58" s="45" t="s">
         <v>561</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="45" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F59" s="19" t="s">
+      <c r="F59" s="45" t="s">
         <v>562</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G59" s="45" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F60" s="19" t="s">
+      <c r="F60" s="45" t="s">
         <v>564</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="45" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="45" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="45" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F63" s="19" t="s">
+      <c r="F63" s="45" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F64" s="23" t="s">
+      <c r="F64" s="49" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="65" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="45" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G66" s="19" t="s">
+      <c r="G66" s="45" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G67" s="19" t="s">
+      <c r="G67" s="45" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="68" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G68" s="19" t="s">
+      <c r="G68" s="45" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="69" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F69" s="23" t="s">
+      <c r="F69" s="49" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="70" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="45" t="s">
         <v>688</v>
       </c>
-      <c r="F70" s="23"/>
+      <c r="F70" s="49"/>
     </row>
     <row r="71" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F71" s="23" t="s">
+      <c r="F71" s="49" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F72" s="23" t="s">
+      <c r="F72" s="49" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="73" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F73" s="23" t="s">
+      <c r="F73" s="49" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="74" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F74" s="23" t="s">
+      <c r="F74" s="49" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="75" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F75" s="23" t="s">
+      <c r="F75" s="49" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D76" s="24" t="s">
+      <c r="D76" s="50" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="77" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E77" s="52" t="s">
+      <c r="E77" s="45" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="78" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="45" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="79" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F79" s="19" t="s">
+      <c r="F79" s="45" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="80" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F80" s="19" t="s">
+      <c r="F80" s="45" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="81" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F81" s="19" t="s">
+      <c r="F81" s="45" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="82" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F82" s="19" t="s">
+      <c r="F82" s="45" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="83" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E83" s="19" t="s">
+      <c r="E83" s="45" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="84" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="45" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="85" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="45" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="86" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="45" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="87" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F87" s="19" t="s">
+      <c r="F87" s="45" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="88" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F88" s="19" t="s">
+      <c r="F88" s="45" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="89" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E89" s="19" t="s">
+      <c r="E89" s="45" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="90" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E90" s="19" t="s">
+      <c r="E90" s="45" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="91" spans="5:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E91" s="53" t="s">
+    <row r="91" spans="5:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E91" s="51" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="92" spans="5:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F92" s="53" t="s">
+    <row r="92" spans="5:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F92" s="51" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="93" spans="5:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G93" s="53" t="s">
+    <row r="93" spans="5:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G93" s="51" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="94" spans="5:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F94" s="53" t="s">
+    <row r="94" spans="5:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F94" s="51" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="95" spans="5:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G95" s="53" t="s">
+    <row r="95" spans="5:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G95" s="51" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="96" spans="5:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H96" s="53" t="s">
+    <row r="96" spans="5:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H96" s="51" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="97" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G97" s="53" t="s">
+    <row r="97" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G97" s="51" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="98" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G98" s="53"/>
-      <c r="H98" s="53" t="s">
+    <row r="98" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H98" s="51" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="99" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G99" s="53" t="s">
+    <row r="99" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G99" s="51" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="100" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F100" s="53" t="s">
+    <row r="100" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F100" s="51" t="s">
         <v>737</v>
       </c>
-      <c r="G100" s="53"/>
-    </row>
-    <row r="101" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F101" s="53"/>
-      <c r="G101" s="53" t="s">
+    </row>
+    <row r="101" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G101" s="51" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="102" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F102" s="53"/>
-      <c r="G102" s="53"/>
-      <c r="H102" s="53" t="s">
+    <row r="102" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H102" s="51" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="103" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F103" s="53"/>
-      <c r="G103" s="53" t="s">
+    <row r="103" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G103" s="51" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="104" spans="3:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F104" s="53"/>
-      <c r="G104" s="53"/>
-      <c r="H104" s="53" t="s">
+    <row r="104" spans="3:8" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H104" s="51" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="105" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C105" s="20" t="s">
+      <c r="C105" s="46" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="106" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D106" s="19" t="s">
+      <c r="D106" s="45" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="107" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D107" s="19" t="s">
+      <c r="D107" s="45" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="108" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D108" s="19" t="s">
+      <c r="D108" s="45" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="109" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E109" s="24" t="s">
+      <c r="E109" s="50" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="110" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D110" s="19" t="s">
+      <c r="D110" s="45" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="111" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="E111" s="19" t="s">
+      <c r="E111" s="45" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="112" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D112" s="19" t="s">
+      <c r="D112" s="45" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="113" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E113" s="24" t="s">
+      <c r="E113" s="50" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="114" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F114" s="19" t="s">
+      <c r="F114" s="45" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="115" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F115" s="19" t="s">
+      <c r="F115" s="45" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="116" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E116" s="24" t="s">
+      <c r="E116" s="50" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="117" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F117" s="19" t="s">
+      <c r="F117" s="45" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="118" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F118" s="19" t="s">
+      <c r="F118" s="45" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="119" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E119" s="24" t="s">
+      <c r="E119" s="50" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="120" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F120" s="19" t="s">
+      <c r="F120" s="45" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="121" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F121" s="19" t="s">
+      <c r="F121" s="45" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="122" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F122" s="19" t="s">
+      <c r="F122" s="45" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="123" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F123" s="19" t="s">
+      <c r="F123" s="45" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="124" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F124" s="19" t="s">
+      <c r="F124" s="45" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="125" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="G125" s="19" t="s">
+      <c r="G125" s="45" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="126" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="H126" s="19" t="s">
+      <c r="H126" s="45" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="127" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="H127" s="19" t="s">
+      <c r="H127" s="45" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="128" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="G128" s="19" t="s">
+      <c r="G128" s="45" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="129" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H129" s="19" t="s">
+      <c r="H129" s="45" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="130" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H130" s="19" t="s">
+      <c r="H130" s="45" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="131" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H131" s="19" t="s">
+      <c r="H131" s="45" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="132" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I132" s="19" t="s">
+      <c r="I132" s="45" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="133" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J133" s="19" t="s">
+      <c r="J133" s="45" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="134" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J134" s="19" t="s">
+      <c r="J134" s="45" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="135" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J135" s="19" t="s">
+      <c r="J135" s="45" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="136" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J136" s="19" t="s">
+      <c r="J136" s="45" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="137" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="K137" s="19" t="s">
+      <c r="K137" s="45" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="138" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="K138" s="19" t="s">
+      <c r="K138" s="45" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="139" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="L139" s="19" t="s">
+      <c r="L139" s="45" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="140" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I140" s="19" t="s">
+      <c r="I140" s="45" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="141" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J141" s="19" t="s">
+      <c r="J141" s="45" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="142" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J142" s="19" t="s">
+      <c r="J142" s="45" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="143" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J143" s="19" t="s">
+      <c r="J143" s="45" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="144" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J144" s="19" t="s">
+      <c r="J144" s="45" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="J145" s="19" t="s">
+      <c r="J145" s="45" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="146" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="J146" s="19" t="s">
+      <c r="J146" s="45" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="K147" s="19" t="s">
+      <c r="K147" s="45" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="K148" s="19" t="s">
+      <c r="K148" s="45" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="L149" s="19" t="s">
+      <c r="L149" s="45" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="L150" s="19" t="s">
+      <c r="L150" s="45" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="151" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="L151" s="19" t="s">
+      <c r="L151" s="45" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="152" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="E152" s="24" t="s">
+      <c r="E152" s="50" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="F153" s="19" t="s">
+      <c r="F153" s="45" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="F154" s="19" t="s">
+      <c r="F154" s="45" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="F155" s="19" t="s">
+      <c r="F155" s="45" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G156" s="19" t="s">
+      <c r="G156" s="45" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="157" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="F157" s="19" t="s">
+      <c r="F157" s="45" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B159" s="19" t="s">
+      <c r="B159" s="45" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C160" s="19" t="s">
+      <c r="C160" s="45" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="162" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C162" s="19" t="s">
+      <c r="C162" s="45" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="163" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D163" s="19" t="s">
+      <c r="D163" s="45" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="164" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D164" s="19" t="s">
+      <c r="D164" s="45" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D165" s="19" t="s">
+      <c r="D165" s="45" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E166" s="19" t="s">
+      <c r="E166" s="45" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="167" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F167" s="19" t="s">
+      <c r="F167" s="45" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F168" s="19" t="s">
+      <c r="F168" s="45" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="169" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F169" s="19" t="s">
+      <c r="F169" s="45" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="170" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E170" s="19" t="s">
+      <c r="E170" s="45" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="171" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D171" s="19" t="s">
+      <c r="D171" s="45" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="172" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E172" s="19" t="s">
+      <c r="E172" s="45" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="173" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E173" s="19" t="s">
+      <c r="E173" s="45" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F174" s="19" t="s">
+      <c r="F174" s="45" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="175" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F175" s="23" t="s">
+      <c r="F175" s="49" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="176" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="G176" s="19" t="s">
+      <c r="G176" s="45" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="177" spans="1:2" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="178" spans="1:2" s="25" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="18" t="s">
+    <row r="177" spans="1:2" s="47" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="178" spans="1:2" s="52" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="44" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B179" s="19" t="s">
+      <c r="B179" s="45" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B181" s="19" t="s">
+      <c r="B181" s="45" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B182" s="23" t="s">
+      <c r="B182" s="49" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B183" s="19" t="s">
+      <c r="B183" s="45" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B184" s="23" t="s">
+      <c r="B184" s="49" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B185" s="19" t="s">
+      <c r="B185" s="45" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B186" s="23" t="s">
+      <c r="B186" s="49" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B187" s="19" t="s">
+      <c r="B187" s="45" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B188" s="23" t="s">
+      <c r="B188" s="49" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B189" s="19" t="s">
+      <c r="B189" s="45" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B190" s="23" t="s">
+      <c r="B190" s="49" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B191" s="19" t="s">
+      <c r="B191" s="45" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B193" s="19" t="s">
+      <c r="B193" s="45" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B194" s="19" t="s">
+      <c r="B194" s="45" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B195" s="19" t="s">
+      <c r="B195" s="45" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B196" s="19" t="s">
+      <c r="B196" s="45" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B197" s="19" t="s">
+      <c r="B197" s="45" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B198" s="19" t="s">
+      <c r="B198" s="45" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B199" s="19" t="s">
+      <c r="B199" s="45" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B200" s="19" t="s">
+      <c r="B200" s="45" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B201" s="19" t="s">
+      <c r="B201" s="45" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B202" s="19" t="s">
+      <c r="B202" s="45" t="s">
         <v>647</v>
       </c>
     </row>

</xml_diff>